<commit_message>
Add algorithm to create a tiles Levels
- add scheme to create levels i exel file
</commit_message>
<xml_diff>
--- a/bunny/Game/Levels/legend_level.xlsx
+++ b/bunny/Game/Levels/legend_level.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
   </bookViews>
   <sheets>
-    <sheet name="Zeszyt1" sheetId="1" r:id="rId1"/>
+    <sheet name="legend_level" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1019,7 +1019,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15744265" y="5367619"/>
+          <a:off x="15744265" y="4941794"/>
           <a:ext cx="627529" cy="627529"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1826,7 +1826,7 @@
   <dimension ref="A1:CW40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="O13" sqref="O12:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Initialize ladder collisions begin
</commit_message>
<xml_diff>
--- a/bunny/Game/Levels/legend_level.xlsx
+++ b/bunny/Game/Levels/legend_level.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2024" uniqueCount="25">
   <si>
     <t>002</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>000</t>
+  </si>
+  <si>
+    <t>111</t>
   </si>
 </sst>
 </file>
@@ -1557,6 +1560,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>563870</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>104429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Obraz 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9681882" y="7676030"/>
+          <a:ext cx="563870" cy="563870"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1826,7 +1873,7 @@
   <dimension ref="A1:CW40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O13" sqref="O12:O13"/>
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -9451,7 +9498,9 @@
         <v>108</v>
       </c>
       <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
+      <c r="Q33" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="R33" s="3"/>
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>

</xml_diff>